<commit_message>
modify template to make it generic
</commit_message>
<xml_diff>
--- a/csv/trello_template.xlsx
+++ b/csv/trello_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/holmgmat/Documents/projects/Rotakorn/trello_csv_export/csv/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/holmgmat/Documents/projects/personal-projects/trello_csv_export/csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF7FFC09-799E-D048-9BDB-F3243702D685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB7625E-A902-BA47-93F9-1A8816EBE826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4920" yWindow="1960" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Name</t>
   </si>
@@ -33,38 +33,6 @@
   <si>
     <t>Labels</t>
   </si>
-  <si>
-    <t>Nicklas</t>
-  </si>
-  <si>
-    <t>Tobbe</t>
-  </si>
-  <si>
-    <t>Philip</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Prioritering</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">                           Notera prioritet nedan.  1-5</t>
-    </r>
-  </si>
 </sst>
 </file>
 
@@ -215,7 +183,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -401,20 +369,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="15">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -529,75 +485,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -643,7 +530,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -667,19 +554,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -736,133 +610,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>419101</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>19051</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BD5DA42-D1FE-773E-EB0F-125BC82C1478}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="17164051" y="10267950"/>
-          <a:ext cx="2038350" cy="2838450"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent4">
-            <a:lumMod val="40000"/>
-            <a:lumOff val="60000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="sv-SE" sz="1100"/>
-            <a:t>Prio 1: Högst</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="sv-SE" sz="1100" baseline="0"/>
-            <a:t> prio, fokusera snarast.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="sv-SE" sz="1100" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="sv-SE" sz="1100" baseline="0"/>
-            <a:t>Prio 2: Väldigt intressant men gör 1:orna först. </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="sv-SE" sz="1100" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="sv-SE" sz="1100" baseline="0"/>
-            <a:t>Prio 3: Detta vill absolut lägga tid på men "inte nu". </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="sv-SE" sz="1100" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="sv-SE" sz="1100" baseline="0"/>
-            <a:t>Prio 4: Relevant men avvakta.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="sv-SE" sz="1100" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="sv-SE" sz="1100" baseline="0"/>
-            <a:t>Prio 5: Borde vi inte ta bort detta? </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="sv-SE" sz="1100" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="sv-SE" sz="1100" baseline="0"/>
-            <a:t>Ingen åsikt: Lämna blankt.</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1162,12 +909,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J68"/>
+  <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="J19" sqref="J19"/>
+      <selection pane="bottomLeft" activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1178,10 +925,9 @@
     <col min="5" max="5" width="32.1640625" style="2" customWidth="1"/>
     <col min="6" max="6" width="3.83203125" style="3" customWidth="1"/>
     <col min="7" max="7" width="4.5" customWidth="1"/>
-    <col min="8" max="8" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8"/>
       <c r="B1" s="4" t="s">
         <v>2</v>
@@ -1196,365 +942,209 @@
         <v>3</v>
       </c>
       <c r="F1" s="7"/>
-      <c r="H1" s="13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C2" s="1"/>
-      <c r="H2" s="9"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C3" s="1"/>
-      <c r="H3" s="9"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C4" s="1"/>
-      <c r="H4" s="9"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C5" s="1"/>
-      <c r="H5" s="9"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C6" s="1"/>
-      <c r="H6" s="9"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C7" s="1"/>
-      <c r="H7" s="9"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C8" s="1"/>
-      <c r="H8" s="9"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C9" s="1"/>
-      <c r="H9" s="9"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C10" s="1"/>
-      <c r="H10" s="9"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H11" s="9"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C12" s="1"/>
-      <c r="H12" s="9"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C13" s="1"/>
-      <c r="H13" s="9"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C14" s="1"/>
-      <c r="H14" s="9"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C15" s="1"/>
-      <c r="H15" s="9"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C16" s="1"/>
-      <c r="H16" s="9"/>
-    </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C17" s="1"/>
-      <c r="H17" s="9"/>
-    </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C18" s="1"/>
-      <c r="H18" s="9"/>
-    </row>
-    <row r="19" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C19" s="1"/>
-      <c r="H19" s="9"/>
-    </row>
-    <row r="20" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C20" s="1"/>
-      <c r="H20" s="9"/>
-    </row>
-    <row r="21" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C21" s="1"/>
-      <c r="H21" s="9"/>
-    </row>
-    <row r="22" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C22" s="1"/>
-      <c r="H22" s="9"/>
-    </row>
-    <row r="23" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C23" s="1"/>
-      <c r="H23" s="9"/>
-    </row>
-    <row r="24" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C24" s="1"/>
-      <c r="H24" s="9"/>
-    </row>
-    <row r="25" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C25" s="1"/>
-      <c r="H25" s="9"/>
-    </row>
-    <row r="26" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C26" s="1"/>
-      <c r="H26" s="9"/>
-    </row>
-    <row r="27" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C27" s="1"/>
-      <c r="H27" s="9"/>
-    </row>
-    <row r="28" spans="3:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C28" s="1"/>
-      <c r="H28" s="9"/>
-    </row>
-    <row r="29" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C29" s="1"/>
-      <c r="H29" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="I29" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J29" s="12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C30" s="1"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
-    </row>
-    <row r="31" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C31" s="1"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10"/>
-    </row>
-    <row r="32" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C32" s="1"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="10"/>
-    </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C33" s="1"/>
-      <c r="H33" s="10"/>
-      <c r="I33" s="10"/>
-      <c r="J33" s="10"/>
-    </row>
-    <row r="34" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C34" s="1"/>
-      <c r="H34" s="10"/>
-      <c r="I34" s="10"/>
-      <c r="J34" s="10"/>
-    </row>
-    <row r="35" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C35" s="1"/>
-      <c r="H35" s="10"/>
-      <c r="I35" s="10"/>
-      <c r="J35" s="10"/>
-    </row>
-    <row r="36" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C36" s="1"/>
-      <c r="H36" s="10"/>
-      <c r="I36" s="10"/>
-      <c r="J36" s="10"/>
-    </row>
-    <row r="37" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C37" s="1"/>
-      <c r="H37" s="10"/>
-      <c r="I37" s="10"/>
-      <c r="J37" s="10"/>
-    </row>
-    <row r="38" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C38" s="1"/>
-      <c r="H38" s="10"/>
-      <c r="I38" s="10"/>
-      <c r="J38" s="10"/>
-    </row>
-    <row r="39" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C39" s="1"/>
-      <c r="H39" s="10"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="10"/>
-    </row>
-    <row r="40" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C40" s="1"/>
-      <c r="H40" s="10"/>
-      <c r="I40" s="10"/>
-      <c r="J40" s="10"/>
-    </row>
-    <row r="41" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C41" s="1"/>
-      <c r="H41" s="10"/>
-      <c r="I41" s="10"/>
-      <c r="J41" s="10"/>
-    </row>
-    <row r="42" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C42" s="1"/>
-      <c r="H42" s="10"/>
-      <c r="I42" s="10"/>
-      <c r="J42" s="10"/>
-    </row>
-    <row r="43" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C43" s="1"/>
-      <c r="H43" s="10"/>
-      <c r="I43" s="10"/>
-      <c r="J43" s="10"/>
-    </row>
-    <row r="44" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C44" s="1"/>
-      <c r="H44" s="10"/>
-      <c r="I44" s="10"/>
-      <c r="J44" s="10"/>
-    </row>
-    <row r="45" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C45" s="1"/>
-      <c r="H45" s="10"/>
-      <c r="I45" s="10"/>
-      <c r="J45" s="10"/>
-    </row>
-    <row r="46" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C46" s="1"/>
-      <c r="H46" s="10"/>
-      <c r="I46" s="10"/>
-      <c r="J46" s="10"/>
-    </row>
-    <row r="47" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C47" s="1"/>
-      <c r="H47" s="10"/>
-      <c r="I47" s="10"/>
-      <c r="J47" s="10"/>
-    </row>
-    <row r="48" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C48" s="1"/>
-      <c r="H48" s="10"/>
-      <c r="I48" s="10"/>
-      <c r="J48" s="10"/>
-    </row>
-    <row r="49" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C49" s="1"/>
-      <c r="H49" s="10"/>
-      <c r="I49" s="10"/>
-      <c r="J49" s="10"/>
-    </row>
-    <row r="50" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C50" s="1"/>
-      <c r="H50" s="10"/>
-      <c r="I50" s="10"/>
-      <c r="J50" s="10"/>
-    </row>
-    <row r="51" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C51" s="1"/>
-      <c r="H51" s="10"/>
-      <c r="I51" s="10"/>
-      <c r="J51" s="10"/>
-    </row>
-    <row r="52" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C52" s="1"/>
-      <c r="H52" s="10"/>
-      <c r="I52" s="10"/>
-      <c r="J52" s="10"/>
-    </row>
-    <row r="53" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C53" s="1"/>
-      <c r="H53" s="10"/>
-      <c r="I53" s="10"/>
-      <c r="J53" s="10"/>
-    </row>
-    <row r="54" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C54" s="1"/>
-      <c r="H54" s="10"/>
-      <c r="I54" s="10"/>
-      <c r="J54" s="10"/>
-    </row>
-    <row r="55" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C55" s="1"/>
-      <c r="H55" s="10"/>
-      <c r="I55" s="10"/>
-      <c r="J55" s="10"/>
-    </row>
-    <row r="56" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C56" s="1"/>
-      <c r="H56" s="10"/>
-      <c r="I56" s="10"/>
-      <c r="J56" s="10"/>
-    </row>
-    <row r="57" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C57" s="1"/>
-      <c r="H57" s="10"/>
-      <c r="I57" s="10"/>
-      <c r="J57" s="10"/>
-    </row>
-    <row r="58" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C58" s="1"/>
-      <c r="H58" s="10"/>
-      <c r="I58" s="10"/>
-      <c r="J58" s="10"/>
-    </row>
-    <row r="59" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C59" s="1"/>
-      <c r="H59" s="10"/>
-      <c r="I59" s="10"/>
-      <c r="J59" s="10"/>
-    </row>
-    <row r="60" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C60" s="1"/>
-      <c r="H60" s="10"/>
-      <c r="I60" s="10"/>
-      <c r="J60" s="10"/>
-    </row>
-    <row r="61" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C61" s="1"/>
-      <c r="H61" s="10"/>
-      <c r="I61" s="10"/>
-      <c r="J61" s="10"/>
-    </row>
-    <row r="62" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C62" s="1"/>
-      <c r="H62" s="10"/>
-      <c r="I62" s="10"/>
-      <c r="J62" s="10"/>
-    </row>
-    <row r="63" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C63" s="1"/>
-      <c r="H63" s="10"/>
-      <c r="I63" s="10"/>
-      <c r="J63" s="10"/>
-    </row>
-    <row r="64" spans="3:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C64" s="1"/>
-      <c r="H64" s="10"/>
-      <c r="I64" s="10"/>
-      <c r="J64" s="10"/>
-    </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C65" s="1"/>
-      <c r="H65" s="10"/>
-      <c r="I65" s="10"/>
-      <c r="J65" s="10"/>
-    </row>
-    <row r="66" spans="2:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B66"/>
       <c r="C66"/>
       <c r="E66"/>
       <c r="F66"/>
-      <c r="H66" s="10"/>
-      <c r="I66" s="10"/>
-      <c r="J66" s="10"/>
-    </row>
-    <row r="67" spans="2:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B67"/>
-      <c r="H67" s="11"/>
-      <c r="I67" s="11"/>
-      <c r="J67" s="11"/>
-    </row>
-    <row r="68" spans="2:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B68"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>